<commit_message>
Problems for day 2
</commit_message>
<xml_diff>
--- a/problems.xlsx
+++ b/problems.xlsx
@@ -389,9 +389,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H79" sqref="H79"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -518,7 +516,7 @@
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -532,7 +530,7 @@
         <v>2</v>
       </c>
       <c r="D10" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -546,7 +544,7 @@
         <v>3</v>
       </c>
       <c r="D11" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -574,7 +572,7 @@
         <v>5</v>
       </c>
       <c r="D13" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -588,7 +586,7 @@
         <v>6</v>
       </c>
       <c r="D14" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -616,7 +614,7 @@
         <v>8</v>
       </c>
       <c r="D16" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1078,7 +1076,7 @@
         <v>1</v>
       </c>
       <c r="D49" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -1106,7 +1104,7 @@
         <v>3</v>
       </c>
       <c r="D51" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -1120,7 +1118,7 @@
         <v>4</v>
       </c>
       <c r="D52" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -1134,7 +1132,7 @@
         <v>5</v>
       </c>
       <c r="D53" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -1162,7 +1160,7 @@
         <v>7</v>
       </c>
       <c r="D55" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -1176,7 +1174,7 @@
         <v>8</v>
       </c>
       <c r="D56" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -1638,7 +1636,7 @@
         <v>1</v>
       </c>
       <c r="D89" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
@@ -1652,7 +1650,7 @@
         <v>2</v>
       </c>
       <c r="D90" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
@@ -1680,7 +1678,7 @@
         <v>4</v>
       </c>
       <c r="D92" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
@@ -1694,7 +1692,7 @@
         <v>5</v>
       </c>
       <c r="D93" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
@@ -1708,7 +1706,7 @@
         <v>6</v>
       </c>
       <c r="D94" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
@@ -1722,7 +1720,7 @@
         <v>7</v>
       </c>
       <c r="D95" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
@@ -1736,7 +1734,7 @@
         <v>8</v>
       </c>
       <c r="D96" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>